<commit_message>
Fixed bugs, zone_id page_sources added
</commit_message>
<xml_diff>
--- a/mythicplus_tww.xlsx
+++ b/mythicplus_tww.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="99">
   <si>
     <t>Dungeon</t>
   </si>
@@ -43,9 +42,6 @@
     <t>Frontal</t>
   </si>
   <si>
-    <t>Bewildered Pollen</t>
-  </si>
-  <si>
     <t>Success</t>
   </si>
   <si>
@@ -286,9 +282,6 @@
     <t>Comet Storm</t>
   </si>
   <si>
-    <t>Frozen Bindings</t>
-  </si>
-  <si>
     <t>Exile</t>
   </si>
   <si>
@@ -314,6 +307,12 @@
   </si>
   <si>
     <t>AbilityName</t>
+  </si>
+  <si>
+    <t>Bewildering Pollen</t>
+  </si>
+  <si>
+    <t>Frozen Binds</t>
   </si>
 </sst>
 </file>
@@ -695,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -720,7 +719,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>1</v>
@@ -735,16 +734,16 @@
         <v>4</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -767,7 +766,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="H2" s="1">
         <v>321968</v>
@@ -776,7 +775,7 @@
         <v>-1</v>
       </c>
       <c r="J2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -790,16 +789,16 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="H3" s="1">
         <v>322486</v>
@@ -808,7 +807,7 @@
         <v>959842</v>
       </c>
       <c r="J3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -828,10 +827,10 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="H4" s="1">
         <v>324909</v>
@@ -840,7 +839,7 @@
         <v>-1</v>
       </c>
       <c r="J4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -860,10 +859,10 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
         <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
       </c>
       <c r="H5">
         <v>324923</v>
@@ -872,7 +871,7 @@
         <v>-1</v>
       </c>
       <c r="J5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -883,19 +882,19 @@
         <v>13338</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="H6" s="1">
         <v>323138</v>
@@ -904,7 +903,7 @@
         <v>-1</v>
       </c>
       <c r="J6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -915,7 +914,7 @@
         <v>13339</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>2</v>
@@ -924,10 +923,10 @@
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="H7" s="1">
         <v>328756</v>
@@ -936,7 +935,7 @@
         <v>-1</v>
       </c>
       <c r="J7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -947,7 +946,7 @@
         <v>13340</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>2</v>
@@ -956,10 +955,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="H8" s="1">
         <v>323149</v>
@@ -968,7 +967,7 @@
         <v>-1</v>
       </c>
       <c r="J8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -979,19 +978,19 @@
         <v>13341</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" t="s">
         <v>24</v>
-      </c>
-      <c r="G9" t="s">
-        <v>25</v>
       </c>
       <c r="H9">
         <v>323059</v>
@@ -1000,7 +999,7 @@
         <v>-1</v>
       </c>
       <c r="J9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1011,7 +1010,7 @@
         <v>13342</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>2</v>
@@ -1023,7 +1022,7 @@
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10">
         <v>340300</v>
@@ -1032,7 +1031,7 @@
         <v>-1</v>
       </c>
       <c r="J10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1043,7 +1042,7 @@
         <v>13343</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>2</v>
@@ -1055,7 +1054,7 @@
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H11">
         <v>340160</v>
@@ -1064,7 +1063,7 @@
         <v>-1</v>
       </c>
       <c r="J11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1075,7 +1074,7 @@
         <v>13344</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>2</v>
@@ -1084,10 +1083,10 @@
         <v>0</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H12">
         <v>340279</v>
@@ -1096,7 +1095,7 @@
         <v>-1</v>
       </c>
       <c r="J12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1107,7 +1106,7 @@
         <v>13345</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>2</v>
@@ -1116,10 +1115,10 @@
         <v>0</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" t="s">
         <v>30</v>
-      </c>
-      <c r="G13" t="s">
-        <v>31</v>
       </c>
       <c r="H13">
         <v>340305</v>
@@ -1128,7 +1127,7 @@
         <v>-1</v>
       </c>
       <c r="J13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1139,7 +1138,7 @@
         <v>13346</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>2</v>
@@ -1148,10 +1147,10 @@
         <v>0</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" t="s">
         <v>32</v>
-      </c>
-      <c r="G14" t="s">
-        <v>33</v>
       </c>
       <c r="H14">
         <v>340189</v>
@@ -1160,7 +1159,7 @@
         <v>-1</v>
       </c>
       <c r="J14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1171,7 +1170,7 @@
         <v>13347</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>2</v>
@@ -1180,10 +1179,10 @@
         <v>0</v>
       </c>
       <c r="F15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" t="s">
         <v>34</v>
-      </c>
-      <c r="G15" t="s">
-        <v>35</v>
       </c>
       <c r="H15">
         <v>324776</v>
@@ -1192,7 +1191,7 @@
         <v>-1</v>
       </c>
       <c r="J15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1203,19 +1202,19 @@
         <v>13348</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="2">
         <v>0</v>
       </c>
       <c r="F16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" t="s">
         <v>36</v>
-      </c>
-      <c r="G16" t="s">
-        <v>37</v>
       </c>
       <c r="H16">
         <v>324776</v>
@@ -1224,7 +1223,7 @@
         <v>136006</v>
       </c>
       <c r="J16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1235,7 +1234,7 @@
         <v>13349</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>2</v>
@@ -1244,10 +1243,10 @@
         <v>0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H17" s="1">
         <v>324914</v>
@@ -1256,7 +1255,7 @@
         <v>-1</v>
       </c>
       <c r="J17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1267,7 +1266,7 @@
         <v>13351</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>2</v>
@@ -1276,10 +1275,10 @@
         <v>0</v>
       </c>
       <c r="F18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="H18" s="4">
         <v>341709</v>
@@ -1288,7 +1287,7 @@
         <v>-1</v>
       </c>
       <c r="J18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1299,19 +1298,19 @@
         <v>13352</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19" s="2">
         <v>0</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="H19" s="1">
         <v>321828</v>
@@ -1320,7 +1319,7 @@
         <v>134470</v>
       </c>
       <c r="J19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1331,7 +1330,7 @@
         <v>13353</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>2</v>
@@ -1340,10 +1339,10 @@
         <v>0</v>
       </c>
       <c r="F20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="H20" s="4">
         <v>336499</v>
@@ -1352,7 +1351,7 @@
         <v>-1</v>
       </c>
       <c r="J20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1363,19 +1362,19 @@
         <v>13354</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="H21" s="1">
         <v>326046</v>
@@ -1384,7 +1383,7 @@
         <v>-1</v>
       </c>
       <c r="J21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1395,7 +1394,7 @@
         <v>13355</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>2</v>
@@ -1404,10 +1403,10 @@
         <v>0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H22" s="2">
         <v>326021</v>
@@ -1416,7 +1415,7 @@
         <v>-1</v>
       </c>
       <c r="J22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1427,19 +1426,19 @@
         <v>13356</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="H23" s="2">
         <v>337235</v>
@@ -1448,7 +1447,7 @@
         <v>-1</v>
       </c>
       <c r="J23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1459,19 +1458,19 @@
         <v>13357</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E24" s="2">
         <v>0</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="H24" s="1">
         <v>337235</v>
@@ -1480,7 +1479,7 @@
         <v>656595</v>
       </c>
       <c r="J24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1491,7 +1490,7 @@
         <v>13358</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>2</v>
@@ -1500,10 +1499,10 @@
         <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H25" s="2">
         <v>337249</v>
@@ -1512,7 +1511,7 @@
         <v>-1</v>
       </c>
       <c r="J25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1523,19 +1522,19 @@
         <v>13359</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E26" s="2">
         <v>0</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H26" s="1">
         <v>337249</v>
@@ -1544,7 +1543,7 @@
         <v>656595</v>
       </c>
       <c r="J26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1555,7 +1554,7 @@
         <v>13360</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>2</v>
@@ -1564,10 +1563,10 @@
         <v>0</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H27" s="2">
         <v>337255</v>
@@ -1576,7 +1575,7 @@
         <v>-1</v>
       </c>
       <c r="J27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1587,19 +1586,19 @@
         <v>13361</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E28" s="2">
         <v>0</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H28" s="1">
         <v>337255</v>
@@ -1608,7 +1607,7 @@
         <v>656595</v>
       </c>
       <c r="J28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1619,7 +1618,7 @@
         <v>13362</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>2</v>
@@ -1628,10 +1627,10 @@
         <v>0</v>
       </c>
       <c r="F29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="H29" s="1">
         <v>322614</v>
@@ -1640,7 +1639,7 @@
         <v>-1</v>
       </c>
       <c r="J29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="9" customFormat="1" ht="15.75" thickBot="1">
@@ -1651,7 +1650,7 @@
         <v>13364</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>2</v>
@@ -1660,10 +1659,10 @@
         <v>0</v>
       </c>
       <c r="F30" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="H30" s="9">
         <v>322550</v>
@@ -1672,50 +1671,50 @@
         <v>-1</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="1">
+        <v>12917</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="1">
-        <v>12916</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" s="2">
-        <v>0</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="G31" s="1" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="H31" s="1">
-        <v>321968</v>
+        <v>320596</v>
       </c>
       <c r="I31" s="1">
         <v>-1</v>
       </c>
       <c r="J31" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="1">
-        <v>12917</v>
+        <v>12918</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>2</v>
@@ -1723,66 +1722,66 @@
       <c r="E32" s="2">
         <v>0</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G32" s="1" t="s">
+      <c r="F32" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H32" s="1">
-        <v>320596</v>
-      </c>
-      <c r="I32" s="1">
+      <c r="G32" t="s">
+        <v>64</v>
+      </c>
+      <c r="H32">
+        <v>320631</v>
+      </c>
+      <c r="I32" s="4">
         <v>-1</v>
       </c>
       <c r="J32" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" s="1">
-        <v>12918</v>
+        <v>12919</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E33" s="2">
         <v>0</v>
       </c>
       <c r="F33" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" t="s">
         <v>64</v>
-      </c>
-      <c r="G33" t="s">
-        <v>65</v>
       </c>
       <c r="H33">
         <v>320631</v>
       </c>
-      <c r="I33" s="4">
-        <v>-1</v>
+      <c r="I33" s="1">
+        <v>136030</v>
       </c>
       <c r="J33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B34" s="1">
-        <v>12919</v>
+        <v>12920</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E34" s="2">
         <v>0</v>
@@ -1791,27 +1790,27 @@
         <v>66</v>
       </c>
       <c r="G34" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H34">
-        <v>320631</v>
+        <v>324293</v>
       </c>
       <c r="I34" s="1">
-        <v>136030</v>
+        <v>-1</v>
       </c>
       <c r="J34" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B35" s="1">
-        <v>12920</v>
+        <v>12921</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>2</v>
@@ -1820,30 +1819,30 @@
         <v>0</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="G35" t="s">
         <v>68</v>
       </c>
       <c r="H35">
-        <v>324293</v>
-      </c>
-      <c r="I35" s="1">
+        <v>324323</v>
+      </c>
+      <c r="I35" s="4">
         <v>-1</v>
       </c>
       <c r="J35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B36" s="1">
-        <v>12921</v>
+        <v>12922</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>2</v>
@@ -1852,158 +1851,158 @@
         <v>0</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G36" t="s">
         <v>69</v>
       </c>
       <c r="H36">
-        <v>324323</v>
+        <v>335141</v>
       </c>
       <c r="I36" s="4">
-        <v>-1</v>
+        <v>2576096</v>
       </c>
       <c r="J36" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37" s="1">
-        <v>12922</v>
+        <v>12923</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E37" s="2">
         <v>0</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="G37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H37">
         <v>335141</v>
       </c>
       <c r="I37" s="4">
-        <v>2576096</v>
+        <v>-1</v>
       </c>
       <c r="J37" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B38" s="1">
-        <v>12923</v>
+        <v>12924</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E38" s="2">
         <v>0</v>
       </c>
       <c r="F38" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" t="s">
         <v>71</v>
       </c>
-      <c r="G38" t="s">
-        <v>70</v>
-      </c>
       <c r="H38">
-        <v>335141</v>
+        <v>345623</v>
       </c>
       <c r="I38" s="4">
         <v>-1</v>
       </c>
       <c r="J38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B39" s="1">
-        <v>12924</v>
+        <v>12925</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E39" s="2">
         <v>0</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="G39" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H39">
-        <v>345623</v>
+        <v>324372</v>
       </c>
       <c r="I39" s="4">
         <v>-1</v>
       </c>
       <c r="J39" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B40" s="1">
-        <v>12925</v>
+        <v>12926</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="E40" s="2">
         <v>0</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="G40" t="s">
         <v>74</v>
       </c>
       <c r="H40">
-        <v>324372</v>
+        <v>324387</v>
       </c>
       <c r="I40" s="4">
         <v>-1</v>
       </c>
       <c r="J40" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B41" s="1">
-        <v>12926</v>
+        <v>12927</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>2</v>
@@ -2012,126 +2011,126 @@
         <v>0</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>17</v>
+        <v>75</v>
       </c>
       <c r="G41" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H41">
-        <v>324387</v>
+        <v>333488</v>
       </c>
       <c r="I41" s="4">
         <v>-1</v>
       </c>
       <c r="J41" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B42" s="1">
-        <v>12927</v>
+        <v>12928</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E42" s="2">
         <v>0</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G42" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H42">
-        <v>333488</v>
+        <v>320012</v>
       </c>
       <c r="I42" s="4">
-        <v>-1</v>
+        <v>136224</v>
       </c>
       <c r="J42" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B43" s="1">
-        <v>12928</v>
+        <v>12929</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E43" s="2">
         <v>0</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="G43" t="s">
         <v>79</v>
       </c>
       <c r="H43">
-        <v>320012</v>
+        <v>321226</v>
       </c>
       <c r="I43" s="4">
-        <v>136224</v>
+        <v>-1</v>
       </c>
       <c r="J43" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B44" s="1">
-        <v>12929</v>
+        <v>12930</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="E44" s="2">
         <v>0</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="G44" t="s">
         <v>80</v>
       </c>
       <c r="H44">
-        <v>321226</v>
+        <v>338353</v>
       </c>
       <c r="I44" s="4">
         <v>-1</v>
       </c>
       <c r="J44" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B45" s="1">
-        <v>12930</v>
+        <v>12931</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>2</v>
@@ -2140,30 +2139,30 @@
         <v>0</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="G45" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H45">
-        <v>338353</v>
+        <v>338606</v>
       </c>
       <c r="I45" s="4">
         <v>-1</v>
       </c>
       <c r="J45" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B46" s="1">
-        <v>12931</v>
+        <v>12932</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>2</v>
@@ -2172,94 +2171,94 @@
         <v>0</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="G46" t="s">
         <v>83</v>
       </c>
       <c r="H46">
-        <v>338606</v>
+        <v>333477</v>
       </c>
       <c r="I46" s="4">
         <v>-1</v>
       </c>
       <c r="J46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B47" s="1">
-        <v>12932</v>
+        <v>12933</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E47" s="2">
         <v>0</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="G47" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H47">
-        <v>333477</v>
+        <v>322681</v>
       </c>
       <c r="I47" s="4">
         <v>-1</v>
       </c>
       <c r="J47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B48" s="1">
-        <v>12933</v>
+        <v>12934</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="E48" s="2">
         <v>0</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G48" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H48">
-        <v>322681</v>
+        <v>343556</v>
       </c>
       <c r="I48" s="4">
         <v>-1</v>
       </c>
       <c r="J48" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B49" s="1">
-        <v>12934</v>
+        <v>12935</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>2</v>
@@ -2268,30 +2267,30 @@
         <v>0</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="G49" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="H49">
-        <v>343556</v>
+        <v>320772</v>
       </c>
       <c r="I49" s="4">
         <v>-1</v>
       </c>
       <c r="J49" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B50" s="1">
-        <v>12935</v>
+        <v>12936</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>2</v>
@@ -2300,30 +2299,30 @@
         <v>0</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="G50" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="H50">
-        <v>320784</v>
+        <v>320788</v>
       </c>
       <c r="I50" s="4">
         <v>-1</v>
       </c>
       <c r="J50" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B51" s="1">
-        <v>12936</v>
+        <v>12937</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>2</v>
@@ -2332,51 +2331,19 @@
         <v>0</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="G51" t="s">
         <v>89</v>
       </c>
       <c r="H51">
-        <v>320788</v>
+        <v>321894</v>
       </c>
       <c r="I51" s="4">
         <v>-1</v>
       </c>
       <c r="J51" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
-      <c r="A52" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B52" s="1">
-        <v>12937</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E52" s="2">
-        <v>0</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G52" t="s">
-        <v>91</v>
-      </c>
-      <c r="H52">
-        <v>321894</v>
-      </c>
-      <c r="I52" s="4">
-        <v>-1</v>
-      </c>
-      <c r="J52" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Big WIP, code for scraping warcraftlogs
</commit_message>
<xml_diff>
--- a/mythicplus_tww.xlsx
+++ b/mythicplus_tww.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="116">
   <si>
     <t>Dungeon</t>
   </si>
@@ -313,6 +313,57 @@
   </si>
   <si>
     <t>Frozen Binds</t>
+  </si>
+  <si>
+    <t>Grim Batol</t>
+  </si>
+  <si>
+    <t>Umbral Wind</t>
+  </si>
+  <si>
+    <t>Mass Tremor</t>
+  </si>
+  <si>
+    <t>Commanding Roar</t>
+  </si>
+  <si>
+    <t>Molten Mace</t>
+  </si>
+  <si>
+    <t>Kite Boss</t>
+  </si>
+  <si>
+    <t>Fiery Cleave</t>
+  </si>
+  <si>
+    <t>Ascension</t>
+  </si>
+  <si>
+    <t>Twilight Buffet</t>
+  </si>
+  <si>
+    <t>Knockback</t>
+  </si>
+  <si>
+    <t>Devouring Flame</t>
+  </si>
+  <si>
+    <t>Invocation of Shadowflame</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Shadow Gale</t>
+  </si>
+  <si>
+    <t>Hide</t>
+  </si>
+  <si>
+    <t>Void Infusion</t>
+  </si>
+  <si>
+    <t>Dodge Airstrikes</t>
   </si>
 </sst>
 </file>
@@ -373,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -400,6 +451,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -694,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -707,7 +759,7 @@
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" customWidth="1"/>
     <col min="5" max="5" width="3.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="21.85546875" customWidth="1"/>
     <col min="8" max="8" width="8.42578125" customWidth="1"/>
     <col min="9" max="9" width="8" customWidth="1"/>
@@ -2314,35 +2366,288 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:10" s="9" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A51" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="6">
         <v>12937</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E51" s="2">
-        <v>0</v>
-      </c>
-      <c r="F51" s="4" t="s">
+      <c r="D51" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E51" s="8">
+        <v>0</v>
+      </c>
+      <c r="F51" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G51" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="9">
         <v>321894</v>
       </c>
-      <c r="I51" s="4">
-        <v>-1</v>
-      </c>
-      <c r="J51" t="s">
+      <c r="I51" s="7">
+        <v>-1</v>
+      </c>
+      <c r="J51" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G52" t="s">
+        <v>100</v>
+      </c>
+      <c r="H52">
+        <v>451939</v>
+      </c>
+      <c r="J52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G53" t="s">
+        <v>101</v>
+      </c>
+      <c r="H53">
+        <v>451871</v>
+      </c>
+      <c r="J53" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G54" t="s">
+        <v>102</v>
+      </c>
+      <c r="H54">
+        <v>448847</v>
+      </c>
+      <c r="J54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G55" t="s">
+        <v>103</v>
+      </c>
+      <c r="H55">
+        <v>449687</v>
+      </c>
+      <c r="J55" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" t="s">
+        <v>105</v>
+      </c>
+      <c r="H56">
+        <v>447395</v>
+      </c>
+      <c r="J56" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G57" t="s">
+        <v>106</v>
+      </c>
+      <c r="H57">
+        <v>451387</v>
+      </c>
+      <c r="J57" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G58" t="s">
+        <v>107</v>
+      </c>
+      <c r="H58">
+        <v>456751</v>
+      </c>
+      <c r="J58" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" t="s">
+        <v>109</v>
+      </c>
+      <c r="H59">
+        <v>448105</v>
+      </c>
+      <c r="J59" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G60" t="s">
+        <v>110</v>
+      </c>
+      <c r="H60">
+        <v>448013</v>
+      </c>
+      <c r="J60" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G61" t="s">
+        <v>112</v>
+      </c>
+      <c r="H61">
+        <v>449939</v>
+      </c>
+      <c r="J61" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G62" t="s">
+        <v>114</v>
+      </c>
+      <c r="H62">
+        <v>450088</v>
+      </c>
+      <c r="J62" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>